<commit_message>
readworkboox and test 3
</commit_message>
<xml_diff>
--- a/input_for_generator/geneinfo.xlsx
+++ b/input_for_generator/geneinfo.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
+    <t xml:space="preserve">geneid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geneid</t>
   </si>
   <si>
     <t xml:space="preserve">lenght</t>
@@ -139,8 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,7 +168,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,20 +176,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.77"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>